<commit_message>
legend and code refactor
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Projects/statistica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FE079B-CFE2-A946-9714-20B98C6E7316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382294AC-240F-624A-8EA5-43CA086B2799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16140" xr2:uid="{9BF8877F-7556-4642-8BD7-1B4C86FF5A46}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9BF8877F-7556-4642-8BD7-1B4C86FF5A46}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,124 +36,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Data</t>
   </si>
   <si>
-    <t>Cecha 1</t>
-  </si>
-  <si>
-    <t>Cecha 2</t>
-  </si>
-  <si>
-    <t>Cecha 3</t>
-  </si>
-  <si>
-    <t>Cecha 4</t>
-  </si>
-  <si>
-    <t>Cecha 5</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:30:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:31:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:32:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:33:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:34:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:35:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:36:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:37:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:38:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:39:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:40:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:41:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:42:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:43:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:44:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:45:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:46:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:47:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:48:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:49:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:50:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:51:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:52:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:53:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:54:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:55:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:56:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:57:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:58:00.000Z</t>
-  </si>
-  <si>
-    <t>2023-11-03T14:59:00.000Z</t>
+    <t>2000-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2001-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2002-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2003-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2004-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2005-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2006-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2007-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2008-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2009-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2010-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2011-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2012-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2013-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2014-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2015-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2016-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2017-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2018-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2019-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2020-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>Cars total</t>
+  </si>
+  <si>
+    <t>2021-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>2022-01-01T00:00:00</t>
+  </si>
+  <si>
+    <t>Passenger cars</t>
+  </si>
+  <si>
+    <t>Trucks</t>
+  </si>
+  <si>
+    <t>Buses</t>
+  </si>
+  <si>
+    <t>Motorcycles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -496,15 +481,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB70F588-0072-DA48-B9D8-DCCF442FE80D}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -512,622 +499,483 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>42</v>
+        <v>14106000</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>9991000</v>
       </c>
       <c r="D2">
-        <v>56</v>
+        <v>1879000</v>
       </c>
       <c r="E2">
-        <v>32</v>
+        <v>82000</v>
       </c>
       <c r="F2">
-        <v>79</v>
+        <v>803000</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>14724000</v>
       </c>
       <c r="C3">
-        <v>91</v>
+        <v>10503000</v>
       </c>
       <c r="D3">
-        <v>23</v>
+        <v>1979000</v>
       </c>
       <c r="E3">
-        <v>57</v>
+        <v>82000</v>
       </c>
       <c r="F3">
-        <v>84</v>
+        <v>803000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>73</v>
+        <v>15525000</v>
       </c>
       <c r="C4">
-        <v>49</v>
+        <v>11029000</v>
       </c>
       <c r="D4">
-        <v>63</v>
+        <v>2163000</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>83000</v>
       </c>
       <c r="F4">
-        <v>70</v>
+        <v>869000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>15899000</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>11244000</v>
       </c>
       <c r="D5">
-        <v>69</v>
+        <v>2313000</v>
       </c>
       <c r="E5">
-        <v>96</v>
+        <v>83000</v>
       </c>
       <c r="F5">
-        <v>58</v>
+        <v>845000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>16701000</v>
       </c>
       <c r="C6">
-        <v>82</v>
+        <v>11975000</v>
       </c>
       <c r="D6">
-        <v>44</v>
+        <v>2392000</v>
       </c>
       <c r="E6">
-        <v>27</v>
+        <v>83000</v>
       </c>
       <c r="F6">
-        <v>66</v>
+        <v>836000</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>16815923</v>
       </c>
       <c r="C7">
-        <v>77</v>
+        <v>12339000</v>
       </c>
       <c r="D7">
-        <v>75</v>
+        <v>2305000</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>80000</v>
       </c>
       <c r="F7">
-        <v>99</v>
+        <v>754000</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>26</v>
+        <v>18035047</v>
       </c>
       <c r="C8">
-        <v>67</v>
+        <v>13384000</v>
       </c>
       <c r="D8">
-        <v>88</v>
+        <v>2393000</v>
       </c>
       <c r="E8">
-        <v>53</v>
+        <v>84000</v>
       </c>
       <c r="F8">
-        <v>24</v>
+        <v>784000</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>94</v>
+        <v>19471836</v>
       </c>
       <c r="C9">
-        <v>60</v>
+        <v>14588739</v>
       </c>
       <c r="D9">
-        <v>53</v>
+        <v>2520548</v>
       </c>
       <c r="E9">
-        <v>85</v>
+        <v>87586</v>
       </c>
       <c r="F9">
-        <v>35</v>
+        <v>825305</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>21336913</v>
       </c>
       <c r="C10">
-        <v>38</v>
+        <v>16079533</v>
       </c>
       <c r="D10">
-        <v>41</v>
+        <v>2709697</v>
       </c>
       <c r="E10">
-        <v>59</v>
+        <v>92401</v>
       </c>
       <c r="F10">
-        <v>14</v>
+        <v>909144</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>80</v>
+        <v>22024697</v>
       </c>
       <c r="C11">
-        <v>45</v>
+        <v>16494650.000000002</v>
       </c>
       <c r="D11">
-        <v>72</v>
+        <v>2796767.0000000005</v>
       </c>
       <c r="E11">
-        <v>11</v>
+        <v>95415</v>
       </c>
       <c r="F11">
-        <v>68</v>
+        <v>974906</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>46</v>
+        <v>23037149</v>
       </c>
       <c r="C12">
-        <v>51</v>
+        <v>17239800</v>
       </c>
       <c r="D12">
-        <v>76</v>
+        <v>2981616</v>
       </c>
       <c r="E12">
-        <v>65</v>
+        <v>97044</v>
       </c>
       <c r="F12">
-        <v>29</v>
+        <v>1013014</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>36</v>
+        <v>24189370</v>
       </c>
       <c r="C13">
-        <v>86</v>
+        <v>18125490</v>
       </c>
       <c r="D13">
-        <v>16</v>
+        <v>3130729</v>
       </c>
       <c r="E13">
-        <v>25</v>
+        <v>100299</v>
       </c>
       <c r="F13">
-        <v>54</v>
+        <v>1069195</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>21</v>
+        <v>24875717</v>
       </c>
       <c r="C14">
-        <v>95</v>
+        <v>18744412</v>
       </c>
       <c r="D14">
-        <v>66</v>
+        <v>3178005</v>
       </c>
       <c r="E14">
-        <v>6</v>
+        <v>99858</v>
       </c>
       <c r="F14">
-        <v>10</v>
+        <v>1107260</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>89</v>
+        <v>25683575</v>
       </c>
       <c r="C15">
-        <v>43</v>
+        <v>19389446</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3242484</v>
       </c>
       <c r="E15">
-        <v>97</v>
+        <v>102602</v>
       </c>
       <c r="F15">
-        <v>48</v>
+        <v>1153169</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>81</v>
+        <v>26472274</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>20003863</v>
       </c>
       <c r="D16">
-        <v>33</v>
+        <v>3340616</v>
       </c>
       <c r="E16">
-        <v>71</v>
+        <v>106057</v>
       </c>
       <c r="F16">
-        <v>92</v>
+        <v>1189527</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>62</v>
+        <v>27409106</v>
       </c>
       <c r="C17">
-        <v>47</v>
+        <v>20723423</v>
       </c>
       <c r="D17">
-        <v>9</v>
+        <v>3428882</v>
       </c>
       <c r="E17">
-        <v>37</v>
+        <v>109844</v>
       </c>
       <c r="F17">
-        <v>78</v>
+        <v>1272333</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>22</v>
+        <v>28601037</v>
       </c>
       <c r="C18">
-        <v>55</v>
+        <v>21675388</v>
       </c>
       <c r="D18">
-        <v>40</v>
+        <v>3542279.0000000005</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>113139</v>
       </c>
       <c r="F18">
-        <v>61</v>
+        <v>1355625</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B19">
-        <v>28</v>
+        <v>29634928</v>
       </c>
       <c r="C19">
-        <v>31</v>
+        <v>22503579</v>
       </c>
       <c r="D19">
-        <v>74</v>
+        <v>3639909</v>
       </c>
       <c r="E19">
-        <v>87</v>
+        <v>116090</v>
       </c>
       <c r="F19">
-        <v>50</v>
+        <v>1427115</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B20">
-        <v>64</v>
+        <v>30700890</v>
       </c>
       <c r="C20">
-        <v>52</v>
+        <v>23429016</v>
       </c>
       <c r="D20">
-        <v>28</v>
+        <v>3759140.0000000005</v>
       </c>
       <c r="E20">
-        <v>2</v>
+        <v>119471</v>
       </c>
       <c r="F20">
-        <v>100</v>
+        <v>1502888</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>31989313</v>
       </c>
       <c r="C21">
-        <v>34</v>
+        <v>24360166</v>
       </c>
       <c r="D21">
-        <v>64</v>
+        <v>3884472</v>
       </c>
       <c r="E21">
-        <v>93</v>
+        <v>122604</v>
       </c>
       <c r="F21">
-        <v>83</v>
+        <v>1587031</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B22">
-        <v>59</v>
+        <v>32991083</v>
       </c>
       <c r="C22">
-        <v>67</v>
+        <v>25113862</v>
       </c>
       <c r="D22">
-        <v>95</v>
+        <v>4009154</v>
       </c>
       <c r="E22">
-        <v>81</v>
+        <v>124526</v>
       </c>
       <c r="F22">
-        <v>8</v>
+        <v>1669138</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>34030267</v>
       </c>
       <c r="C23">
-        <v>45</v>
+        <v>25869804</v>
       </c>
       <c r="D23">
-        <v>49</v>
+        <v>4140804</v>
       </c>
       <c r="E23">
-        <v>76</v>
+        <v>126547</v>
       </c>
       <c r="F23">
-        <v>70</v>
+        <v>1749697</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>27</v>
+        <v>34866137</v>
       </c>
       <c r="C24">
-        <v>84</v>
+        <v>26457659</v>
       </c>
       <c r="D24">
-        <v>47</v>
+        <v>4251226</v>
       </c>
       <c r="E24">
-        <v>90</v>
+        <v>128677</v>
       </c>
       <c r="F24">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25">
-        <v>68</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-      <c r="D25">
-        <v>68</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="F25">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26">
-        <v>22</v>
-      </c>
-      <c r="C26">
-        <v>82</v>
-      </c>
-      <c r="D26">
-        <v>85</v>
-      </c>
-      <c r="E26">
-        <v>61</v>
-      </c>
-      <c r="F26">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27">
-        <v>38</v>
-      </c>
-      <c r="C27">
-        <v>74</v>
-      </c>
-      <c r="D27">
-        <v>21</v>
-      </c>
-      <c r="E27">
-        <v>79</v>
-      </c>
-      <c r="F27">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>77</v>
-      </c>
-      <c r="C28">
-        <v>20</v>
-      </c>
-      <c r="D28">
-        <v>54</v>
-      </c>
-      <c r="E28">
-        <v>36</v>
-      </c>
-      <c r="F28">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29">
-        <v>73</v>
-      </c>
-      <c r="C29">
-        <v>88</v>
-      </c>
-      <c r="D29">
-        <v>58</v>
-      </c>
-      <c r="E29">
-        <v>94</v>
-      </c>
-      <c r="F29">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30">
-        <v>91</v>
-      </c>
-      <c r="C30">
-        <v>12</v>
-      </c>
-      <c r="D30">
-        <v>39</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31">
-        <v>50</v>
-      </c>
-      <c r="C31">
-        <v>23</v>
-      </c>
-      <c r="D31">
-        <v>62</v>
-      </c>
-      <c r="E31">
-        <v>55</v>
-      </c>
-      <c r="F31">
-        <v>9</v>
+        <v>1830963</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>